<commit_message>
Progress Bar & Ajax Refresh List
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Raymonds+Thane+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Raymonds+Thane+Ad+Advertiser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,38 +454,40 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Visit Raymond Thane - Consult an expert &amp; visit site
+Launching 2 BHK in Thane West - Homes in Pokhran Rd by...
+raymondtenxera.com
+https://www.raymondtenxera.com › official-site › brand
+New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities. Experience a futuristic lifestyle with Raymond Realty's Spacious 2 BHK homes...</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Raymond Limited</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Address By GS Thane - Consult an expert &amp; visit site
 raymonds-addressbygs.com
 https://www.raymonds-addressbygs.com
-Bookings Open Raymond Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site. Booking Open For Limited Time...
-Price ₹ / BHK/ Area · View Pricing · View The Gallery · Site &amp; Layout Plan · Grand Amenities</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+Bookings Open Addres By GS Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site. Booking Open For Limited Time Only, Sign Up &amp; Get Instant Call Back Now. Early Buy Discount.
+View Pricing · Price ₹ / BHK/ Area · View The Gallery · Site &amp; Layout Plan · Grand Amenities
+2 Bhk - 615 Sq. Ft. - ₹1.61 - Price In Cr
+ · 
+More</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Home Bazaar Services Pvt Ltd</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sponsored
-Launching 2 BHK in Thane West | Homes in Pokhran Rd by...
-raymondtenxera.com
-https://www.raymondtenxera.com › official-site › brand
-New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities. Experience a futuristic lifestyle with Raymond Realty's Spacious 2 BHK homes in Thane West. Library &amp; Reading Lounges.
-Location Map · Location Advantages · About Us · Overview · Configuration · Contact Us</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Raymond Limited</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,62 +500,356 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-Launching The Address By GS | 3/4/4.5 BHK Homes ₹2.59 Cr*
+La Vie at Uptown Urbania | 2&amp;3 BHK at ₹1.49 Cr (All Incl)
+Rustomjee La-Vie
+https://www.rustomjee-lavie.com
+Book 2 &amp; 3 BHK homes from ₹1.49 Cr (All Incl) at Rustomjee La Vie, Thane (W) 2&amp;3BHK from ₹1.49 Cr (All Incl) at Rustomjee La Vie. Pay 20% Now &amp; Nothing Till Jan'25. Luxury flats. Leisure zones.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Kapstone Construction Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane | 3, 4 &amp; 4.5 BHK ₹2.59Cr*
 theaddressbygs-thane.in
 https://www.theaddressbygs-thane.in
-Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now. 2 High Rise Towers. 3-Acres Gated Development. 51 Habitable Floors &amp; Lifestyle Amenities. Schedule A Site Visit. Get Quote. Site &amp; Floor Plans. Request Brochure.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Prop Solutions4u</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Sponsored
 TenX Habitat Thane Launch | 2, 3 &amp; 4 BHK Starts @ 1.41Cr*
 homesfy-property.co.in
 https://www.homesfy-property.co.in › tenx › thane
+326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR* Launching Tenx Habitat at Thane. Lavish 2, 3 &amp; 4 BHK Starting At 1.41Cr* Highlights: Chat Option Available, Floor Plan Available, Brochure Available.
+Price Plan · Our Price · Browse Prices · Floor Plans · Floor Plan · View Gallery</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Homesfy Realty Limited</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sponsored
+Launching Final Tower Asteria
+luxeoffplans.com
+https://www.luxeoffplans.com
+2, 3 &amp; 4 BHK Apartments — Spacious 2, 3 &amp; 4 BHK Homes at Thane. Sample Flat Ready. Download Brochure. Explore Project Details, Speak To Site Expert, Know More.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RABS NET SOLUTIONS PVT LTD</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sponsored
+Exclusive Offers On Site
+raymondsrealtythane.com
+https://www.raymondsrealtythane.com
+Book Online Presentation Today — Luxurious 2, 3, 4 &amp; 4.5 BHK Starts At ₹ 1.30 Cr All Inc | Flexi Payment Plan Available. The Address By GS 2.0 Offers Luxurious 2, 3, 4 &amp; 4.5 BHK Home With Balcony. Pay Just 20% Now. Book a free Site Visit. Easy Payment Plan. Amenities: Senior Citizen Area, Yoga Path.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>zuber khan</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane - 3, 4 &amp; 4.5 BHK ₹2.59Cr*
+theaddressbygs-thane.in
+https://www.theaddressbygs-thane.in
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.
+Call us</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prop Solutions4u</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Address Tower Thane - Consult an expert &amp; visit site
+raymonds-addressbygs.com
+https://www.raymonds-addressbygs.com
+Bookings Open Addres Tower Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Home Bazaar Services Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sponsored
+TenX Habitat Thane Launch - Zero Stamp Duty Offer
+homesfy-property.co.in
+https://www.homesfy-property.co.in › tenx › thane
 326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR*</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Homesfy Realty Limited</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Sponsored
-RTMI Flats with Zero GST* | Grand Clubhouse @Raymond TenX
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sponsored
+La Vie at Uptown Urbania - 2&amp;3 BHK at ₹1.49 Cr (All Incl)
+Rustomjee La-Vie
+https://www.rustomjee-lavie.com
+Book 2 &amp; 3 BHK homes from ₹1.49 Cr (All Incl) at Rustomjee La Vie, Thane (W...</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Kapstone Construction Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sponsored
+TenX Habitat Thane - Zero Stamp Duty Offer
+homesfy-property.co.in
+https://www.homesfy-property.co.in › tenx › thane
+326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR*</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Homesfy Realty Limited</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Pokhran Road | 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.in
+https://www.theaddressbygs-thane.in
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Prop Solutions4u</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Address Tower Thane | Get expert advice &amp; visit site
+raymonds-addressbygs.com
+https://www.raymonds-addressbygs.com
+Bookings Open Addres Tower Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Home Bazaar Services Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Sponsored
+Thane's Finest Homes @Thane | Ready World Class Amenities
+raymondsrealtythane.com
+https://www.raymondsrealtythane.com
+Luxurious 2, 3, 4 &amp; 4.5 BHK Starts At ₹ 1.30 Cr All Inc | Flexi Payment Plan Available. The...</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>zuber khan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sponsored
+2 BHK with Balcony at Raymond - Presenting Homes in Thane...
+raymondtenxera.com
+https://www.raymondtenxera.com › official-site › brand
+New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Raymond Limited</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sponsored
+TenX Habitat Thane | Zero Stamp Duty Offer
+homesfy-property.co.in
+https://www.homesfy-property.co.in › tenx › thane
+326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR*</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Homesfy Realty Limited</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane | 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.in
+https://www.theaddressbygs-thane.in
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Prop Solutions4u</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sponsored
+RTMI Flats with Zero GST* - Grand Clubhouse @Raymond TenX
 tenxhabitatraymondrealty.com
 https://www.tenxhabitatraymondrealty.com
-4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym. Book your 2 BHK Flat in Thane and get 50...
-Real Estate Builders &amp; Construction Company · Thane · Open ⋅ Closes 6 pm
-Floor Plan · Floorplans Section · Configurations Section · Location · View Gallery · Amenities</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Raymond Limited</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>India</t>
         </is>

</xml_diff>

<commit_message>
dashboard pie chart Update with getRefreshList
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Raymonds+Thane+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Raymonds+Thane+Ad+Advertiser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,58 +454,59 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-RTMI Flats with Zero GST* - TenX Habitat by Raymond Realty
-tenxhabitatraymondrealty.com
-https://www.tenxhabitatraymondrealty.com
-4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym. Book your 2 BHK Flat in Thane and get 50+ World-Class Amenities &amp; 270° Panoramic City...</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Raymond Limited</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sponsored
-La Vie at Uptown Urbania | 2&amp;3 BHK at ₹1.49 Cr (All Incl)
-rustomjee-lavie.com
-https://www.rustomjee-lavie.com › rustomjee › official-site
-Book 2 &amp; 3 BHK homes from ₹1.49 Cr (All Incl) at Rustomjee La Vie, Thane (W) 2&amp;3BHK from ₹1.49 Cr (All Incl) at Rustomjee La Vie.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Kapstone Construction Pvt Ltd</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Sponsored
-The Address By GS Thane | 3, 4, 4.5 BHK Price ₹2.59Cr*
+The Address By GS Thane | 3, 4, 4.5 BHK Starts ₹2.59 Cr*
 theaddressbygs-thane.in
 https://www.theaddressbygs-thane.in
 Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.
 Floor Plan &amp; Pricing · Location · Project Highlights · Amenities Offered</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Prop Solutions4u</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Address Tower Thane | Consult an expert &amp; visit site
+raymonds-addressbygs.com
+https://www.raymonds-addressbygs.com
+Bookings Open Addres Tower Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site. Booking Open For Limited Time Only, Sign Up &amp; Get Instant Call Back Now.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Home Bazaar Services Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sponsored
+Launching 2 BHK in Thane West | Pay 20% &amp; Nothing till Jan'25
+raymondtenxera.com
+https://www.raymondtenxera.com › thane › project
+New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities
+Configuration · Overview · Location Map · View Amenities · About Us · Location Advantages</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Prop Solutions4u</t>
+          <t>Raymond Limited</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -518,214 +519,249 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Sponsored
-Visit Address By GS Thane | Consult an expert &amp; visit site
+The Address By GS Thane | 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.ainewprojects.in
+https://theaddressbygs-thane.ainewprojects.in › raymond_realty › new_launch
+The Address by GS at PokhranRoad Thane is a large gated community Pricing Starts ₹2.59Cr*.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Asset India Realty</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sponsored
+La Vie at Uptown Urbania - 2&amp;3 BHK at ₹1.49 Cr (All Incl)
+Rustomjee La-Vie
+https://www.rustomjee-lavie.com
+Book 2 &amp; 3 BHK homes from ₹1.49 Cr (All Incl) at Rustomjee La Vie, Thane (W) 2&amp;3BHK from ₹1.49 Cr (All Incl) at Rustomjee La Vie. Pay 20% Now &amp; Nothing Till Jan'25. Luxury flats. Leisure zones. Recreational amenities.
+Gallery · Get Best Offer · Contact Us · About Us</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kapstone Construction Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Tower At Thane | Booking Open, Sale ON Save Now
+housebazaar.com
+https://www.housebazaar.com › launch_offer
+Bookings Open Tower At Thane 6.1 Acre, 2/3/4 Bhk ₹ 1.30 Cr Ask Expert &amp; Visit Site. Booking Open For Limited Time Only, Sign Up...
+Price ₹ / BHK/ Area · pricing Details · View The Gallery · Project Overview · Grand Amenities
+2 BHK - 516 Sq.ft. - ₹1.30 - Price In Cr
+ · 
+More</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Home Bazaar Services Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane - 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.ainewprojects.in
+https://theaddressbygs-thane.ainewprojects.in › raymond_realty › new_launch
+The Address by GS at PokhranRoad Thane is a large gated community Pricing Starts ₹2.59Cr*.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Asset India Realty</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane - 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.in
+https://www.theaddressbygs-thane.in
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prop Solutions4u</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sponsored
+La Vie at Uptown Urbania - 2&amp;3 BHK at ₹1.49 Cr (All Incl)
+Rustomjee La-Vie
+https://www.rustomjee-lavie.com
+Book 2 &amp; 3 BHK homes from ₹1.49 Cr (All Incl) at Rustomjee La Vie, Thane (W...</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Kapstone Construction Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sponsored
+New Launch Projects by Raymond - Pay 20% &amp; Nothing till Jan'25
+raymondtenxera.com
+https://www.raymondtenxera.com › thane › project
+New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities. Experience a futuristic lifestyle with...</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Raymond Limited</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sponsored
+Visit Address Tower Thane - Consult an expert &amp; visit site
 raymonds-addressbygs.com
 https://www.raymonds-addressbygs.com
-Bookings Open Addres By GS Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+Bookings Open Addres Tower Thane 6.1 Acre, 2/3/4 Bhk 1.30 Cr Ask Expert &amp; Visit Site
+View Pricing · Price ₹ / BHK/ Area · Grand Amenities · View The Gallery · Site &amp; Layout Plan
+2 Bhk - 615 Sq. Ft. - ₹1.61 - Price In Cr
+ · 
+More
+Call us</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Home Bazaar Services Pvt Ltd</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Sponsored
-TenX Habitat Thane Launch | 2, 3 &amp; 4 BHK Starts @ 1.41Cr*
-homesfy-property.co.in
-https://www.homesfy-property.co.in › tenx › thane
-326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR* Launching Tenx Habitat at Thane. Lavish 2, 3 &amp; 4 BHK Starting At 1.41Cr*.
-Price Plan · Our Price · Floor Plans · Browse Prices · Floor Plan · Find Location</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Homesfy Realty Limited</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sponsored
-RTMI Homes with Zero GST* - TenX Habitat by Raymond Realty
-tenxhabitatraymondrealty.com
-https://www.tenxhabitatraymondrealty.com
-4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym
-Real Estate Builders &amp; Construction Company · Thane · Open ⋅ Closes 6 pm
-Call us</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Raymond Limited</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sponsored
-TenX Habitat Thane Launch | Zero Stamp Duty Offer
-homesfy-property.co.in
-https://www.homesfy-property.co.in › tenx › thane
-326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR*
-Price Plan · Our Price · Photo Gallery · Browse Prices · Our Gallery · Floor Plans · Floor Plan · Find Location · Search Location · View Amenities</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Homesfy Realty Limited</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sponsored
-The Address By GS Thane | 3/4/4.5 BHK Homes ₹2.59 Cr*
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Pokhran Road - 3, 4 &amp; 4.5 BHK ₹2.59Cr*
 theaddressbygs-thane.in
 https://www.theaddressbygs-thane.in
 Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.
 Call us</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Prop Solutions4u</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sponsored
-The Address By GS Thane - 3, 4 &amp; 4.5 BHK ₹2.59Cr*
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane - 3, 4, 4.5 BHK Price ₹2.59Cr*
+theaddressbygs-thane.ainewprojects.in
+https://theaddressbygs-thane.ainewprojects.in › raymond_realty › new_launch
+The Address by GS at PokhranRoad Thane is a large gated community Pricing Starts ₹2.59Cr*.
+Call us</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Asset India Realty</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sponsored
+The Address By GS Thane - 3, 4, 4.5 BHK Starts ₹2.59 Cr*
 theaddressbygs-thane.in
 https://www.theaddressbygs-thane.in
-Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now. 2 High Rise Towers. 3-Acres Gated Development.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.
+Call us
+Location
+Close to Pokhran Road Connectivity to Major Destinations
+Floor Plan &amp; Pricing
+Enquire For Floor Plan &amp; Pricing Request Price Breakup
+Project Highlights
+2 High Rise Towers 51 Habitable Floors
+Amenities Offered
+Thane's Largest Clubhouse Indoor Games, Kids Play Area</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Prop Solutions4u</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Sponsored
-RTMI Homes with Zero GST* | TenX Habitat by Raymond Realty
-tenxhabitatraymondrealty.com
-https://www.tenxhabitatraymondrealty.com
-4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym
-Real Estate Builders &amp; Construction Company · Thane · Open ⋅ Closes 6 pm</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Raymond Limited</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Sponsored
-TenX Habitat Thane Launch | Zero Stamp Duty Offer
-homesfy-property.co.in
-https://www.homesfy-property.co.in › tenx › thane
-326,500 sq ft clubhouse | 2 and 3 BHK residences near Viviana Mall @ 1.41 CR*</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Homesfy Realty Limited</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Sponsored
-RTMI Homes with Zero GST* | TenX Habitat by Raymond Realty
-tenxhabitatraymondrealty.com
-https://www.tenxhabitatraymondrealty.com
-4,200 Sq.Ft. Multipurpose Hall | 28 Seater Mini Theatre | 2,400 Sq.Ft. Fully Equipped Gym
-Real Estate Builders &amp; Construction Company · Thane · Open ⋅ Closes 6 pm</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Raymond Limited</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Sponsored
-The Address By GS Thane | 3, 4, 4.5 BHK Starts ₹2.59 Cr*
-theaddressbygs-thane.in
-https://www.theaddressbygs-thane.in
-Launching The Address by GS at Pokhran Road Thane. Price Starts at ₹2.59 Cr*. Book Now.</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Prop Solutions4u</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>India</t>
         </is>

</xml_diff>